<commit_message>
minor bug fixes in get_pf_shortcircuit_results.py, added updated pf_bus_sc_results_all_cases.xlsx
</commit_message>
<xml_diff>
--- a/pandapower/test/shortcircuit/SCE_Tests/pf_bus_sc_results_all_cases.xlsx
+++ b/pandapower/test/shortcircuit/SCE_Tests/pf_bus_sc_results_all_cases.xlsx
@@ -79,16 +79,16 @@
     <t>pf_rk0_ohm</t>
   </si>
   <si>
+    <t>pf_xk0_ohm</t>
+  </si>
+  <si>
     <t>pf_rk1_ohm</t>
   </si>
   <si>
-    <t>pf_rk2_ohm</t>
+    <t>pf_xk1_ohm</t>
   </si>
   <si>
-    <t>pf_xk0_ohm</t>
-  </si>
-  <si>
-    <t>pf_xk1_ohm</t>
+    <t>pf_rk2_ohm</t>
   </si>
   <si>
     <t>pf_xk2_ohm</t>
@@ -620,16 +620,16 @@
         <v>0.4428835862221404</v>
       </c>
       <c r="I2">
+        <v>4.40271973851942</v>
+      </c>
+      <c r="J2">
         <v>0.4378163569293868</v>
       </c>
-      <c r="J2">
+      <c r="K2">
+        <v>4.378163482534344</v>
+      </c>
+      <c r="L2">
         <v>0.4378163569022844</v>
-      </c>
-      <c r="K2">
-        <v>4.40271973851942</v>
-      </c>
-      <c r="L2">
-        <v>4.378163482534344</v>
       </c>
       <c r="M2">
         <v>4.378163482487168</v>
@@ -661,16 +661,16 @@
         <v>4.185910274912399</v>
       </c>
       <c r="I3">
+        <v>5.870495034006284</v>
+      </c>
+      <c r="J3">
         <v>0.9578163680532483</v>
       </c>
-      <c r="J3">
+      <c r="K3">
+        <v>4.968163485641733</v>
+      </c>
+      <c r="L3">
         <v>0.9578163680261339</v>
-      </c>
-      <c r="K3">
-        <v>5.870495034006284</v>
-      </c>
-      <c r="L3">
-        <v>4.968163485641733</v>
       </c>
       <c r="M3">
         <v>4.968163485594578</v>
@@ -702,16 +702,16 @@
         <v>7.895175922947225</v>
       </c>
       <c r="I4">
+        <v>7.335082718453467</v>
+      </c>
+      <c r="J4">
         <v>1.477816378918005</v>
       </c>
-      <c r="J4">
+      <c r="K4">
+        <v>5.558163489027947</v>
+      </c>
+      <c r="L4">
         <v>1.477816378890885</v>
-      </c>
-      <c r="K4">
-        <v>7.335082718453467</v>
-      </c>
-      <c r="L4">
-        <v>5.558163489027947</v>
       </c>
       <c r="M4">
         <v>5.558163488980837</v>
@@ -743,16 +743,16 @@
         <v>7.895175922947224</v>
       </c>
       <c r="I5">
+        <v>7.335082718453457</v>
+      </c>
+      <c r="J5">
         <v>1.477816378918004</v>
       </c>
-      <c r="J5">
+      <c r="K5">
+        <v>5.558163489027946</v>
+      </c>
+      <c r="L5">
         <v>1.477816378890884</v>
-      </c>
-      <c r="K5">
-        <v>7.335082718453457</v>
-      </c>
-      <c r="L5">
-        <v>5.558163489027946</v>
       </c>
       <c r="M5">
         <v>5.558163488980837</v>
@@ -838,16 +838,16 @@
         <v>0.5041743431842544</v>
       </c>
       <c r="I2">
+        <v>5.006897135806584</v>
+      </c>
+      <c r="J2">
         <v>0.4975185876946874</v>
       </c>
-      <c r="J2">
+      <c r="K2">
+        <v>4.975185775457811</v>
+      </c>
+      <c r="L2">
         <v>0.4975185877124232</v>
-      </c>
-      <c r="K2">
-        <v>5.006897135806584</v>
-      </c>
-      <c r="L2">
-        <v>4.975185775457811</v>
       </c>
       <c r="M2">
         <v>4.975185775488254</v>
@@ -879,16 +879,16 @@
         <v>7.698542227644789</v>
       </c>
       <c r="I3">
+        <v>6.432196710719398</v>
+      </c>
+      <c r="J3">
         <v>1.495918608642645</v>
       </c>
-      <c r="J3">
+      <c r="K3">
+        <v>5.565185778068525</v>
+      </c>
+      <c r="L3">
         <v>1.495918608660561</v>
-      </c>
-      <c r="K3">
-        <v>6.432196710719398</v>
-      </c>
-      <c r="L3">
-        <v>5.565185778068525</v>
       </c>
       <c r="M3">
         <v>5.565185778099361</v>
@@ -920,16 +920,16 @@
         <v>14.8217784003751</v>
       </c>
       <c r="I4">
+        <v>7.872438169825732</v>
+      </c>
+      <c r="J4">
         <v>2.494318629322498</v>
       </c>
-      <c r="J4">
+      <c r="K4">
+        <v>6.155185781258161</v>
+      </c>
+      <c r="L4">
         <v>2.494318629340454</v>
-      </c>
-      <c r="K4">
-        <v>7.872438169825732</v>
-      </c>
-      <c r="L4">
-        <v>6.155185781258161</v>
       </c>
       <c r="M4">
         <v>6.155185781289154</v>
@@ -961,16 +961,16 @@
         <v>14.82177840037509</v>
       </c>
       <c r="I5">
+        <v>7.872438169825724</v>
+      </c>
+      <c r="J5">
         <v>2.494318629322495</v>
       </c>
-      <c r="J5">
+      <c r="K5">
+        <v>6.155185781258152</v>
+      </c>
+      <c r="L5">
         <v>2.494318629340448</v>
-      </c>
-      <c r="K5">
-        <v>7.872438169825724</v>
-      </c>
-      <c r="L5">
-        <v>6.155185781258152</v>
       </c>
       <c r="M5">
         <v>6.15518578128915</v>
@@ -1056,16 +1056,16 @@
         <v>0.5041743431842544</v>
       </c>
       <c r="I2">
+        <v>5.006897135806584</v>
+      </c>
+      <c r="J2">
         <v>0.4975185876946874</v>
       </c>
-      <c r="J2">
+      <c r="K2">
+        <v>4.975185775457811</v>
+      </c>
+      <c r="L2">
         <v>0.4975185877124232</v>
-      </c>
-      <c r="K2">
-        <v>5.006897135806584</v>
-      </c>
-      <c r="L2">
-        <v>4.975185775457811</v>
       </c>
       <c r="M2">
         <v>4.975185775488254</v>
@@ -1097,16 +1097,16 @@
         <v>7.698542227644789</v>
       </c>
       <c r="I3">
+        <v>6.432196710719398</v>
+      </c>
+      <c r="J3">
         <v>1.495918608642645</v>
       </c>
-      <c r="J3">
+      <c r="K3">
+        <v>5.565185778068525</v>
+      </c>
+      <c r="L3">
         <v>1.495918608660561</v>
-      </c>
-      <c r="K3">
-        <v>6.432196710719398</v>
-      </c>
-      <c r="L3">
-        <v>5.565185778068525</v>
       </c>
       <c r="M3">
         <v>5.565185778099361</v>
@@ -1138,16 +1138,16 @@
         <v>14.8217784003751</v>
       </c>
       <c r="I4">
+        <v>7.872438169825732</v>
+      </c>
+      <c r="J4">
         <v>2.494318629322498</v>
       </c>
-      <c r="J4">
+      <c r="K4">
+        <v>6.155185781258161</v>
+      </c>
+      <c r="L4">
         <v>2.494318629340454</v>
-      </c>
-      <c r="K4">
-        <v>7.872438169825732</v>
-      </c>
-      <c r="L4">
-        <v>6.155185781258161</v>
       </c>
       <c r="M4">
         <v>6.155185781289154</v>
@@ -1179,16 +1179,16 @@
         <v>14.82177840037509</v>
       </c>
       <c r="I5">
+        <v>7.872438169825724</v>
+      </c>
+      <c r="J5">
         <v>2.494318629322495</v>
       </c>
-      <c r="J5">
+      <c r="K5">
+        <v>6.155185781258152</v>
+      </c>
+      <c r="L5">
         <v>2.494318629340448</v>
-      </c>
-      <c r="K5">
-        <v>7.872438169825724</v>
-      </c>
-      <c r="L5">
-        <v>6.155185781258152</v>
       </c>
       <c r="M5">
         <v>6.15518578128915</v>
@@ -1274,16 +1274,16 @@
         <v>0.4428835862221607</v>
       </c>
       <c r="I2">
+        <v>4.402719738519057</v>
+      </c>
+      <c r="J2">
         <v>0.437816356924225</v>
       </c>
-      <c r="J2">
+      <c r="K2">
+        <v>4.378163482487345</v>
+      </c>
+      <c r="L2">
         <v>0.4378163569023265</v>
-      </c>
-      <c r="K2">
-        <v>4.402719738519057</v>
-      </c>
-      <c r="L2">
-        <v>4.378163482487345</v>
       </c>
       <c r="M2">
         <v>4.378163482487091</v>
@@ -1315,16 +1315,16 @@
         <v>4.185910274912456</v>
       </c>
       <c r="I3">
+        <v>5.870495034005926</v>
+      </c>
+      <c r="J3">
         <v>0.9578163680481669</v>
       </c>
-      <c r="J3">
+      <c r="K3">
+        <v>4.968163485594707</v>
+      </c>
+      <c r="L3">
         <v>0.9578163680263008</v>
-      </c>
-      <c r="K3">
-        <v>5.870495034005926</v>
-      </c>
-      <c r="L3">
-        <v>4.968163485594707</v>
       </c>
       <c r="M3">
         <v>4.968163485594511</v>
@@ -1356,16 +1356,16 @@
         <v>7.895175922947306</v>
       </c>
       <c r="I4">
+        <v>7.335082718453107</v>
+      </c>
+      <c r="J4">
         <v>1.477816378913027</v>
       </c>
-      <c r="J4">
+      <c r="K4">
+        <v>5.558163488980915</v>
+      </c>
+      <c r="L4">
         <v>1.477816378891169</v>
-      </c>
-      <c r="K4">
-        <v>7.335082718453107</v>
-      </c>
-      <c r="L4">
-        <v>5.558163488980915</v>
       </c>
       <c r="M4">
         <v>5.558163488980771</v>
@@ -1397,16 +1397,16 @@
         <v>7.895175922947299</v>
       </c>
       <c r="I5">
+        <v>7.335082718453101</v>
+      </c>
+      <c r="J5">
         <v>1.477816378913028</v>
       </c>
-      <c r="J5">
+      <c r="K5">
+        <v>5.558163488980913</v>
+      </c>
+      <c r="L5">
         <v>1.477816378891169</v>
-      </c>
-      <c r="K5">
-        <v>7.335082718453101</v>
-      </c>
-      <c r="L5">
-        <v>5.558163488980913</v>
       </c>
       <c r="M5">
         <v>5.558163488980769</v>
@@ -1492,16 +1492,16 @@
         <v>0.4428835862221607</v>
       </c>
       <c r="I2">
+        <v>4.402719738519057</v>
+      </c>
+      <c r="J2">
         <v>0.437816356924225</v>
       </c>
-      <c r="J2">
+      <c r="K2">
+        <v>4.378163482487345</v>
+      </c>
+      <c r="L2">
         <v>0.4378163569023265</v>
-      </c>
-      <c r="K2">
-        <v>4.402719738519057</v>
-      </c>
-      <c r="L2">
-        <v>4.378163482487345</v>
       </c>
       <c r="M2">
         <v>4.378163482487091</v>
@@ -1533,16 +1533,16 @@
         <v>4.185910274912456</v>
       </c>
       <c r="I3">
+        <v>5.870495034005926</v>
+      </c>
+      <c r="J3">
         <v>0.9578163680481669</v>
       </c>
-      <c r="J3">
+      <c r="K3">
+        <v>4.968163485594707</v>
+      </c>
+      <c r="L3">
         <v>0.9578163680263008</v>
-      </c>
-      <c r="K3">
-        <v>5.870495034005926</v>
-      </c>
-      <c r="L3">
-        <v>4.968163485594707</v>
       </c>
       <c r="M3">
         <v>4.968163485594511</v>
@@ -1574,16 +1574,16 @@
         <v>7.895175922947306</v>
       </c>
       <c r="I4">
+        <v>7.335082718453107</v>
+      </c>
+      <c r="J4">
         <v>1.477816378913027</v>
       </c>
-      <c r="J4">
+      <c r="K4">
+        <v>5.558163488980915</v>
+      </c>
+      <c r="L4">
         <v>1.477816378891169</v>
-      </c>
-      <c r="K4">
-        <v>7.335082718453107</v>
-      </c>
-      <c r="L4">
-        <v>5.558163488980915</v>
       </c>
       <c r="M4">
         <v>5.558163488980771</v>
@@ -1615,16 +1615,16 @@
         <v>7.895175922947299</v>
       </c>
       <c r="I5">
+        <v>7.335082718453101</v>
+      </c>
+      <c r="J5">
         <v>1.477816378913028</v>
       </c>
-      <c r="J5">
+      <c r="K5">
+        <v>5.558163488980913</v>
+      </c>
+      <c r="L5">
         <v>1.477816378891169</v>
-      </c>
-      <c r="K5">
-        <v>7.335082718453101</v>
-      </c>
-      <c r="L5">
-        <v>5.558163488980913</v>
       </c>
       <c r="M5">
         <v>5.558163488980769</v>
@@ -1710,16 +1710,16 @@
         <v>0.5041743431842567</v>
       </c>
       <c r="I2">
+        <v>5.006897135806157</v>
+      </c>
+      <c r="J2">
         <v>0.4975185876920994</v>
       </c>
-      <c r="J2">
+      <c r="K2">
+        <v>4.975185775488431</v>
+      </c>
+      <c r="L2">
         <v>0.497518587712459</v>
-      </c>
-      <c r="K2">
-        <v>5.006897135806157</v>
-      </c>
-      <c r="L2">
-        <v>4.975185775488431</v>
       </c>
       <c r="M2">
         <v>4.97518577548815</v>
@@ -1751,16 +1751,16 @@
         <v>7.698542227644828</v>
       </c>
       <c r="I3">
+        <v>6.432196710718991</v>
+      </c>
+      <c r="J3">
         <v>1.495918608640806</v>
       </c>
-      <c r="J3">
+      <c r="K3">
+        <v>5.565185778099434</v>
+      </c>
+      <c r="L3">
         <v>1.495918608660816</v>
-      </c>
-      <c r="K3">
-        <v>6.432196710718991</v>
-      </c>
-      <c r="L3">
-        <v>5.565185778099434</v>
       </c>
       <c r="M3">
         <v>5.565185778099255</v>
@@ -1792,16 +1792,16 @@
         <v>14.82177840037519</v>
       </c>
       <c r="I4">
+        <v>7.872438169825329</v>
+      </c>
+      <c r="J4">
         <v>2.494318629320983</v>
       </c>
-      <c r="J4">
+      <c r="K4">
+        <v>6.155185781289128</v>
+      </c>
+      <c r="L4">
         <v>2.494318629340928</v>
-      </c>
-      <c r="K4">
-        <v>7.872438169825329</v>
-      </c>
-      <c r="L4">
-        <v>6.155185781289128</v>
       </c>
       <c r="M4">
         <v>6.155185781289043</v>
@@ -1833,16 +1833,16 @@
         <v>14.82177840037519</v>
       </c>
       <c r="I5">
+        <v>7.872438169825323</v>
+      </c>
+      <c r="J5">
         <v>2.494318629320986</v>
       </c>
-      <c r="J5">
+      <c r="K5">
+        <v>6.155185781289128</v>
+      </c>
+      <c r="L5">
         <v>2.494318629340926</v>
-      </c>
-      <c r="K5">
-        <v>7.872438169825323</v>
-      </c>
-      <c r="L5">
-        <v>6.155185781289128</v>
       </c>
       <c r="M5">
         <v>6.155185781289043</v>
@@ -1928,16 +1928,16 @@
         <v>0.5041743431842567</v>
       </c>
       <c r="I2">
+        <v>5.006897135806157</v>
+      </c>
+      <c r="J2">
         <v>0.4975185876920994</v>
       </c>
-      <c r="J2">
+      <c r="K2">
+        <v>4.975185775488431</v>
+      </c>
+      <c r="L2">
         <v>0.497518587712459</v>
-      </c>
-      <c r="K2">
-        <v>5.006897135806157</v>
-      </c>
-      <c r="L2">
-        <v>4.975185775488431</v>
       </c>
       <c r="M2">
         <v>4.97518577548815</v>
@@ -1969,16 +1969,16 @@
         <v>7.698542227644828</v>
       </c>
       <c r="I3">
+        <v>6.432196710718991</v>
+      </c>
+      <c r="J3">
         <v>1.495918608640806</v>
       </c>
-      <c r="J3">
+      <c r="K3">
+        <v>5.565185778099434</v>
+      </c>
+      <c r="L3">
         <v>1.495918608660816</v>
-      </c>
-      <c r="K3">
-        <v>6.432196710718991</v>
-      </c>
-      <c r="L3">
-        <v>5.565185778099434</v>
       </c>
       <c r="M3">
         <v>5.565185778099255</v>
@@ -2010,16 +2010,16 @@
         <v>14.82177840037519</v>
       </c>
       <c r="I4">
+        <v>7.872438169825329</v>
+      </c>
+      <c r="J4">
         <v>2.494318629320983</v>
       </c>
-      <c r="J4">
+      <c r="K4">
+        <v>6.155185781289128</v>
+      </c>
+      <c r="L4">
         <v>2.494318629340928</v>
-      </c>
-      <c r="K4">
-        <v>7.872438169825329</v>
-      </c>
-      <c r="L4">
-        <v>6.155185781289128</v>
       </c>
       <c r="M4">
         <v>6.155185781289043</v>
@@ -2051,16 +2051,16 @@
         <v>14.82177840037519</v>
       </c>
       <c r="I5">
+        <v>7.872438169825323</v>
+      </c>
+      <c r="J5">
         <v>2.494318629320986</v>
       </c>
-      <c r="J5">
+      <c r="K5">
+        <v>6.155185781289128</v>
+      </c>
+      <c r="L5">
         <v>2.494318629340926</v>
-      </c>
-      <c r="K5">
-        <v>7.872438169825323</v>
-      </c>
-      <c r="L5">
-        <v>6.155185781289128</v>
       </c>
       <c r="M5">
         <v>6.155185781289043</v>
@@ -2440,16 +2440,16 @@
         <v>0.4428835862221396</v>
       </c>
       <c r="I2">
+        <v>4.402719738519417</v>
+      </c>
+      <c r="J2">
         <v>0.4378163569293836</v>
       </c>
-      <c r="J2">
+      <c r="K2">
+        <v>4.378163482534338</v>
+      </c>
+      <c r="L2">
         <v>0.4378163569022834</v>
-      </c>
-      <c r="K2">
-        <v>4.402719738519417</v>
-      </c>
-      <c r="L2">
-        <v>4.378163482534338</v>
       </c>
       <c r="M2">
         <v>4.37816348248716</v>
@@ -2481,16 +2481,16 @@
         <v>4.185910274912402</v>
       </c>
       <c r="I3">
+        <v>5.870495034006279</v>
+      </c>
+      <c r="J3">
         <v>0.957816368053249</v>
       </c>
-      <c r="J3">
+      <c r="K3">
+        <v>4.968163485641724</v>
+      </c>
+      <c r="L3">
         <v>0.957816368026136</v>
-      </c>
-      <c r="K3">
-        <v>5.870495034006279</v>
-      </c>
-      <c r="L3">
-        <v>4.968163485641724</v>
       </c>
       <c r="M3">
         <v>4.968163485594566</v>
@@ -2522,16 +2522,16 @@
         <v>7.895175922947228</v>
       </c>
       <c r="I4">
+        <v>7.33508271845346</v>
+      </c>
+      <c r="J4">
         <v>1.477816378918006</v>
       </c>
-      <c r="J4">
+      <c r="K4">
+        <v>5.558163489027939</v>
+      </c>
+      <c r="L4">
         <v>1.477816378890888</v>
-      </c>
-      <c r="K4">
-        <v>7.33508271845346</v>
-      </c>
-      <c r="L4">
-        <v>5.558163489027939</v>
       </c>
       <c r="M4">
         <v>5.558163488980824</v>
@@ -2563,16 +2563,16 @@
         <v>7.895175922947228</v>
       </c>
       <c r="I5">
+        <v>7.335082718453452</v>
+      </c>
+      <c r="J5">
         <v>1.477816378918005</v>
       </c>
-      <c r="J5">
+      <c r="K5">
+        <v>5.558163489027939</v>
+      </c>
+      <c r="L5">
         <v>1.477816378890889</v>
-      </c>
-      <c r="K5">
-        <v>7.335082718453452</v>
-      </c>
-      <c r="L5">
-        <v>5.558163489027939</v>
       </c>
       <c r="M5">
         <v>5.558163488980824</v>
@@ -2658,16 +2658,16 @@
         <v>0.4428835862221404</v>
       </c>
       <c r="I2">
+        <v>4.40271973851942</v>
+      </c>
+      <c r="J2">
         <v>0.4378163569293868</v>
       </c>
-      <c r="J2">
+      <c r="K2">
+        <v>4.378163482534344</v>
+      </c>
+      <c r="L2">
         <v>0.4378163569022844</v>
-      </c>
-      <c r="K2">
-        <v>4.40271973851942</v>
-      </c>
-      <c r="L2">
-        <v>4.378163482534344</v>
       </c>
       <c r="M2">
         <v>4.378163482487168</v>
@@ -2699,16 +2699,16 @@
         <v>4.185910274912399</v>
       </c>
       <c r="I3">
+        <v>5.870495034006284</v>
+      </c>
+      <c r="J3">
         <v>0.9578163680532483</v>
       </c>
-      <c r="J3">
+      <c r="K3">
+        <v>4.968163485641733</v>
+      </c>
+      <c r="L3">
         <v>0.9578163680261339</v>
-      </c>
-      <c r="K3">
-        <v>5.870495034006284</v>
-      </c>
-      <c r="L3">
-        <v>4.968163485641733</v>
       </c>
       <c r="M3">
         <v>4.968163485594578</v>
@@ -2740,16 +2740,16 @@
         <v>7.895175922947225</v>
       </c>
       <c r="I4">
+        <v>7.335082718453467</v>
+      </c>
+      <c r="J4">
         <v>1.477816378918005</v>
       </c>
-      <c r="J4">
+      <c r="K4">
+        <v>5.558163489027947</v>
+      </c>
+      <c r="L4">
         <v>1.477816378890885</v>
-      </c>
-      <c r="K4">
-        <v>7.335082718453467</v>
-      </c>
-      <c r="L4">
-        <v>5.558163489027947</v>
       </c>
       <c r="M4">
         <v>5.558163488980837</v>
@@ -2781,16 +2781,16 @@
         <v>7.895175922947224</v>
       </c>
       <c r="I5">
+        <v>7.335082718453457</v>
+      </c>
+      <c r="J5">
         <v>1.477816378918004</v>
       </c>
-      <c r="J5">
+      <c r="K5">
+        <v>5.558163489027946</v>
+      </c>
+      <c r="L5">
         <v>1.477816378890884</v>
-      </c>
-      <c r="K5">
-        <v>7.335082718453457</v>
-      </c>
-      <c r="L5">
-        <v>5.558163489027946</v>
       </c>
       <c r="M5">
         <v>5.558163488980837</v>
@@ -2876,16 +2876,16 @@
         <v>0.5041743431842544</v>
       </c>
       <c r="I2">
+        <v>5.006897135806584</v>
+      </c>
+      <c r="J2">
         <v>0.4975185876946874</v>
       </c>
-      <c r="J2">
+      <c r="K2">
+        <v>4.975185775457811</v>
+      </c>
+      <c r="L2">
         <v>0.4975185877124232</v>
-      </c>
-      <c r="K2">
-        <v>5.006897135806584</v>
-      </c>
-      <c r="L2">
-        <v>4.975185775457811</v>
       </c>
       <c r="M2">
         <v>4.975185775488254</v>
@@ -2917,16 +2917,16 @@
         <v>7.698542227644789</v>
       </c>
       <c r="I3">
+        <v>6.432196710719398</v>
+      </c>
+      <c r="J3">
         <v>1.495918608642645</v>
       </c>
-      <c r="J3">
+      <c r="K3">
+        <v>5.565185778068525</v>
+      </c>
+      <c r="L3">
         <v>1.495918608660561</v>
-      </c>
-      <c r="K3">
-        <v>6.432196710719398</v>
-      </c>
-      <c r="L3">
-        <v>5.565185778068525</v>
       </c>
       <c r="M3">
         <v>5.565185778099361</v>
@@ -2958,16 +2958,16 @@
         <v>14.8217784003751</v>
       </c>
       <c r="I4">
+        <v>7.872438169825732</v>
+      </c>
+      <c r="J4">
         <v>2.494318629322498</v>
       </c>
-      <c r="J4">
+      <c r="K4">
+        <v>6.155185781258161</v>
+      </c>
+      <c r="L4">
         <v>2.494318629340454</v>
-      </c>
-      <c r="K4">
-        <v>7.872438169825732</v>
-      </c>
-      <c r="L4">
-        <v>6.155185781258161</v>
       </c>
       <c r="M4">
         <v>6.155185781289154</v>
@@ -2999,16 +2999,16 @@
         <v>14.82177840037509</v>
       </c>
       <c r="I5">
+        <v>7.872438169825724</v>
+      </c>
+      <c r="J5">
         <v>2.494318629322495</v>
       </c>
-      <c r="J5">
+      <c r="K5">
+        <v>6.155185781258152</v>
+      </c>
+      <c r="L5">
         <v>2.494318629340448</v>
-      </c>
-      <c r="K5">
-        <v>7.872438169825724</v>
-      </c>
-      <c r="L5">
-        <v>6.155185781258152</v>
       </c>
       <c r="M5">
         <v>6.15518578128915</v>
@@ -3094,16 +3094,16 @@
         <v>0.5041743431842544</v>
       </c>
       <c r="I2">
+        <v>5.006897135806584</v>
+      </c>
+      <c r="J2">
         <v>0.4975185876946874</v>
       </c>
-      <c r="J2">
+      <c r="K2">
+        <v>4.975185775457811</v>
+      </c>
+      <c r="L2">
         <v>0.4975185877124232</v>
-      </c>
-      <c r="K2">
-        <v>5.006897135806584</v>
-      </c>
-      <c r="L2">
-        <v>4.975185775457811</v>
       </c>
       <c r="M2">
         <v>4.975185775488254</v>
@@ -3135,16 +3135,16 @@
         <v>7.698542227644789</v>
       </c>
       <c r="I3">
+        <v>6.432196710719398</v>
+      </c>
+      <c r="J3">
         <v>1.495918608642645</v>
       </c>
-      <c r="J3">
+      <c r="K3">
+        <v>5.565185778068525</v>
+      </c>
+      <c r="L3">
         <v>1.495918608660561</v>
-      </c>
-      <c r="K3">
-        <v>6.432196710719398</v>
-      </c>
-      <c r="L3">
-        <v>5.565185778068525</v>
       </c>
       <c r="M3">
         <v>5.565185778099361</v>
@@ -3176,16 +3176,16 @@
         <v>14.8217784003751</v>
       </c>
       <c r="I4">
+        <v>7.872438169825732</v>
+      </c>
+      <c r="J4">
         <v>2.494318629322498</v>
       </c>
-      <c r="J4">
+      <c r="K4">
+        <v>6.155185781258161</v>
+      </c>
+      <c r="L4">
         <v>2.494318629340454</v>
-      </c>
-      <c r="K4">
-        <v>7.872438169825732</v>
-      </c>
-      <c r="L4">
-        <v>6.155185781258161</v>
       </c>
       <c r="M4">
         <v>6.155185781289154</v>
@@ -3217,16 +3217,16 @@
         <v>14.82177840037509</v>
       </c>
       <c r="I5">
+        <v>7.872438169825724</v>
+      </c>
+      <c r="J5">
         <v>2.494318629322495</v>
       </c>
-      <c r="J5">
+      <c r="K5">
+        <v>6.155185781258152</v>
+      </c>
+      <c r="L5">
         <v>2.494318629340448</v>
-      </c>
-      <c r="K5">
-        <v>7.872438169825724</v>
-      </c>
-      <c r="L5">
-        <v>6.155185781258152</v>
       </c>
       <c r="M5">
         <v>6.15518578128915</v>
@@ -3312,16 +3312,16 @@
         <v>0.4428835862221404</v>
       </c>
       <c r="I2">
+        <v>4.40271973851942</v>
+      </c>
+      <c r="J2">
         <v>0.4378163569293868</v>
       </c>
-      <c r="J2">
+      <c r="K2">
+        <v>4.378163482534344</v>
+      </c>
+      <c r="L2">
         <v>0.4378163569022844</v>
-      </c>
-      <c r="K2">
-        <v>4.40271973851942</v>
-      </c>
-      <c r="L2">
-        <v>4.378163482534344</v>
       </c>
       <c r="M2">
         <v>4.378163482487168</v>
@@ -3353,16 +3353,16 @@
         <v>4.185910274912399</v>
       </c>
       <c r="I3">
+        <v>5.870495034006284</v>
+      </c>
+      <c r="J3">
         <v>0.9578163680532483</v>
       </c>
-      <c r="J3">
+      <c r="K3">
+        <v>4.968163485641733</v>
+      </c>
+      <c r="L3">
         <v>0.9578163680261339</v>
-      </c>
-      <c r="K3">
-        <v>5.870495034006284</v>
-      </c>
-      <c r="L3">
-        <v>4.968163485641733</v>
       </c>
       <c r="M3">
         <v>4.968163485594578</v>
@@ -3394,16 +3394,16 @@
         <v>7.895175922947225</v>
       </c>
       <c r="I4">
+        <v>7.335082718453467</v>
+      </c>
+      <c r="J4">
         <v>1.477816378918005</v>
       </c>
-      <c r="J4">
+      <c r="K4">
+        <v>5.558163489027947</v>
+      </c>
+      <c r="L4">
         <v>1.477816378890885</v>
-      </c>
-      <c r="K4">
-        <v>7.335082718453467</v>
-      </c>
-      <c r="L4">
-        <v>5.558163489027947</v>
       </c>
       <c r="M4">
         <v>5.558163488980837</v>
@@ -3435,16 +3435,16 @@
         <v>7.895175922947224</v>
       </c>
       <c r="I5">
+        <v>7.335082718453457</v>
+      </c>
+      <c r="J5">
         <v>1.477816378918004</v>
       </c>
-      <c r="J5">
+      <c r="K5">
+        <v>5.558163489027946</v>
+      </c>
+      <c r="L5">
         <v>1.477816378890884</v>
-      </c>
-      <c r="K5">
-        <v>7.335082718453457</v>
-      </c>
-      <c r="L5">
-        <v>5.558163489027946</v>
       </c>
       <c r="M5">
         <v>5.558163488980837</v>

</xml_diff>